<commit_message>
Implement init Account & Employee data
</commit_message>
<xml_diff>
--- a/hr/account/src/main/resources/workbooks/account.xlsx
+++ b/hr/account/src/main/resources/workbooks/account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\marci\hr\account\src\main\resources\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D58101B-F967-4684-8BA9-BD8CBD35ECFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA638FDF-98C4-4FE3-8B5E-B0009C28EFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>email</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>USER</t>
+  </si>
+  <si>
+    <t>1563 Briarwood Drive, Laurel Springs, New Jersey</t>
+  </si>
+  <si>
+    <t>3409 Traders Alley, Kansas City, Missouri</t>
+  </si>
+  <si>
+    <t>1602 Kemper Lane, Salt Lake City, Utah</t>
+  </si>
+  <si>
+    <t>2250 Woodridge Lane, Memphis, Tennessee</t>
   </si>
 </sst>
 </file>
@@ -457,7 +469,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,13 +479,13 @@
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="45.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -535,6 +547,9 @@
       <c r="E3" t="s">
         <v>26</v>
       </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -552,6 +567,9 @@
       <c r="E4" t="s">
         <v>27</v>
       </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -569,6 +587,9 @@
       <c r="E5" t="s">
         <v>27</v>
       </c>
+      <c r="L5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -585,6 +606,9 @@
       </c>
       <c r="E6" t="s">
         <v>27</v>
+      </c>
+      <c r="L6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>